<commit_message>
UTs for train method.
</commit_message>
<xml_diff>
--- a/test/manual_lin_reg.xlsx
+++ b/test/manual_lin_reg.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="96" yWindow="36" windowWidth="10500" windowHeight="5568" activeTab="1"/>
+    <workbookView xWindow="96" yWindow="36" windowWidth="10500" windowHeight="5568"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
   <si>
     <t>x1</t>
   </si>
@@ -52,6 +52,33 @@
   </si>
   <si>
     <t>J</t>
+  </si>
+  <si>
+    <t>Editable Field</t>
+  </si>
+  <si>
+    <t>1. Put the values of x1, x2, and y</t>
+  </si>
+  <si>
+    <t>2. Set the value of ALPHA</t>
+  </si>
+  <si>
+    <t>3. Reset the initial theta values to 0 (row 9)</t>
+  </si>
+  <si>
+    <t>This will recalculate the new thetas and J</t>
+  </si>
+  <si>
+    <t>4. Copy the value of J to the J list in column G to see the J history.</t>
+  </si>
+  <si>
+    <t>5. Copy the new thetas (by value) to the initial thetas.</t>
+  </si>
+  <si>
+    <t>This will trigger another recalculation of new thetas and J.</t>
+  </si>
+  <si>
+    <t>6. Go to step 4</t>
   </si>
 </sst>
 </file>
@@ -67,12 +94,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -87,12 +120,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="4" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -394,20 +429,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.88671875" style="2"/>
     <col min="7" max="7" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -427,123 +462,141 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="3">
         <v>-1.2649999999999999</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="3">
         <v>-1.2649999999999999</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="3">
         <v>290</v>
       </c>
       <c r="E2" s="2">
         <f>$A$9*A2 + $B$9*B2 + $C$9*C2</f>
         <v>-61.13667499999999</v>
       </c>
-      <c r="G2" s="2">
+      <c r="G2" s="4">
         <v>78550</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I2" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="3">
         <v>-0.63200000000000001</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="3">
         <v>-0.63200000000000001</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="3">
         <v>340</v>
       </c>
       <c r="E3" s="2">
         <f>$A$9*A3 + $B$9*B3 + $C$9*C3</f>
         <v>-29.489839999999997</v>
       </c>
-      <c r="G3" s="2">
+      <c r="G3" s="4">
         <v>3267.605</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="3">
         <v>0</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="3">
         <v>0</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="3">
         <v>390</v>
       </c>
       <c r="E4" s="2">
         <f>$A$9*A4 + $B$9*B4 + $C$9*C4</f>
         <v>2.1070000000000002</v>
       </c>
-      <c r="G4" s="2">
+      <c r="G4" s="4">
         <v>144.17833649999949</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>1</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="3">
         <v>0.63200000000000001</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="3">
         <v>0.63200000000000001</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="3">
         <v>440</v>
       </c>
       <c r="E5" s="2">
         <f>$A$9*A5 + $B$9*B5 + $C$9*C5</f>
         <v>33.70384</v>
       </c>
-      <c r="G5" s="2">
+      <c r="G5" s="4">
         <v>14.485168220049896</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>1</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="3">
         <v>1.2649999999999999</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="3">
         <v>1.2649999999999999</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="3">
         <v>490</v>
       </c>
       <c r="E6" s="2">
         <f>$A$9*A6 + $B$9*B6 + $C$9*C6</f>
         <v>65.350674999999995</v>
       </c>
-      <c r="G6" s="2">
+      <c r="G6" s="4">
         <v>8.9974144513511423</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>9</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="3">
         <v>0.01</v>
       </c>
-      <c r="G7" s="2">
+      <c r="G7" s="4">
         <v>8.6640438041331045</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -553,27 +606,38 @@
       <c r="C8" t="s">
         <v>7</v>
       </c>
-      <c r="G8" s="2">
+      <c r="G8" s="4">
         <v>8.5458487490378694</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9">
+      <c r="I8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" s="3">
         <v>2.1070000000000002</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="3">
         <v>18.675999999999998</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="3">
         <v>31.318999999999999</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>5</v>
       </c>
@@ -590,7 +654,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13">
         <f>A$9 - ($B$7/5) * ( ($E$2-$D$2)*A$2 + ($E$3-$D$3)*A$3 + ($E$4-$D$4)*A$4 + ($E$5-$D$5)*A$5 + ($E$6-$D$6)*A$6 )</f>
         <v>5.9859299999999998</v>
@@ -618,7 +682,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>

</xml_diff>